<commit_message>
[Backend] adding imgUrl for project
</commit_message>
<xml_diff>
--- a/document/Plan.xlsx
+++ b/document/Plan.xlsx
@@ -238,11 +238,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,10 +293,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,11 +339,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,10 +361,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -345,21 +414,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -369,75 +423,14 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,7 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,13 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,13 +493,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,25 +583,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,85 +607,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,13 +631,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,6 +822,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -852,6 +848,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,15 +890,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -899,34 +904,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -944,130 +925,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1161,13 +1142,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1837,8 +1818,8 @@
   <sheetPr/>
   <dimension ref="C1:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[Document] update plan & [Backend] update Group entity
</commit_message>
<xml_diff>
--- a/document/Plan.xlsx
+++ b/document/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
   <si>
     <t xml:space="preserve">Project Manager: </t>
   </si>
@@ -652,6 +652,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -676,6 +682,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -730,24 +754,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -775,12 +781,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -799,25 +799,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1363,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T71" sqref="T71:T76"/>
+    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1383,107 +1383,107 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:29">
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="32" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="33" t="s">
+      <c r="AB2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="34"/>
+      <c r="AC2" s="36"/>
     </row>
     <row r="3" spans="3:29">
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="35" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="36"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="38"/>
     </row>
     <row r="4" spans="3:29">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41" t="s">
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="37" t="s">
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="39"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="41"/>
     </row>
     <row r="5" spans="3:29">
       <c r="C5" s="3"/>
@@ -1500,7 +1500,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="32" t="s">
         <v>70</v>
       </c>
       <c r="P5" s="12"/>
@@ -1543,7 +1543,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="79" t="s">
+      <c r="O6" s="32" t="s">
         <v>70</v>
       </c>
       <c r="P6" s="12"/>
@@ -1580,7 +1580,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="79" t="s">
+      <c r="O7" s="32" t="s">
         <v>70</v>
       </c>
       <c r="P7" s="12"/>
@@ -1916,10 +1916,10 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="83" t="s">
+      <c r="P16" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="Q16" s="84"/>
+      <c r="Q16" s="82"/>
       <c r="R16" s="14"/>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -2012,19 +2012,19 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
       <c r="O19" s="13"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="79" t="s">
+      <c r="Q19" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R19" s="14"/>
@@ -2049,19 +2049,19 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
       <c r="O20" s="13"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="80" t="s">
+      <c r="Q20" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R20" s="14"/>
@@ -2086,19 +2086,19 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
       <c r="O21" s="13"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="80" t="s">
+      <c r="Q21" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R21" s="14"/>
@@ -2123,19 +2123,19 @@
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
       <c r="O22" s="13"/>
       <c r="P22" s="14"/>
-      <c r="Q22" s="79" t="s">
+      <c r="Q22" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R22" s="14"/>
@@ -2189,16 +2189,16 @@
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
       <c r="O24" s="13"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="81" t="s">
@@ -2224,16 +2224,16 @@
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="46" t="s">
+      <c r="G25" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
       <c r="O25" s="13"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="81" t="s">
@@ -2259,22 +2259,22 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="46" t="s">
+      <c r="G26" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
       <c r="O26" s="13"/>
       <c r="P26" s="14"/>
-      <c r="Q26" s="83" t="s">
+      <c r="Q26" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="R26" s="84"/>
+      <c r="R26" s="82"/>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
       <c r="U26" s="14"/>
@@ -2296,22 +2296,22 @@
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
       <c r="O27" s="13"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="83" t="s">
+      <c r="Q27" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="R27" s="84"/>
+      <c r="R27" s="82"/>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
       <c r="U27" s="14"/>
@@ -2362,16 +2362,16 @@
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
       <c r="O29" s="13"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
@@ -2399,16 +2399,16 @@
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
       <c r="O30" s="13"/>
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
@@ -2436,16 +2436,16 @@
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
       <c r="O31" s="13"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
@@ -2469,16 +2469,16 @@
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="46" t="s">
+      <c r="G32" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
       <c r="O32" s="13"/>
       <c r="P32" s="14"/>
       <c r="Q32" s="14"/>
@@ -2492,7 +2492,9 @@
       <c r="W32" s="14"/>
       <c r="X32" s="15"/>
       <c r="Y32" s="22"/>
-      <c r="Z32" s="23"/>
+      <c r="Z32" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="AA32" s="23"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="24"/>
@@ -2560,23 +2562,23 @@
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="44" t="s">
+      <c r="G35" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
       <c r="O35" s="13"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="89" t="s">
+      <c r="Q35" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="R35" s="87"/>
-      <c r="S35" s="88"/>
+      <c r="R35" s="88"/>
+      <c r="S35" s="89"/>
       <c r="T35" s="14"/>
       <c r="U35" s="14"/>
       <c r="V35" s="14"/>
@@ -2622,16 +2624,16 @@
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="45" t="s">
+      <c r="G37" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
       <c r="O37" s="13"/>
       <c r="P37" s="14"/>
       <c r="Q37" s="85" t="s">
@@ -2659,16 +2661,16 @@
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="48" t="s">
+      <c r="G38" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="53"/>
       <c r="O38" s="13"/>
       <c r="P38" s="14"/>
       <c r="Q38" s="85" t="s">
@@ -2696,16 +2698,16 @@
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="48" t="s">
+      <c r="G39" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
       <c r="O39" s="13"/>
       <c r="P39" s="14"/>
       <c r="Q39" s="85" t="s">
@@ -2733,31 +2735,33 @@
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="48" t="s">
+      <c r="G40" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="48"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="56"/>
       <c r="O40" s="13"/>
       <c r="P40" s="14"/>
-      <c r="Q40" s="93" t="s">
+      <c r="Q40" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R40" s="91"/>
-      <c r="S40" s="91"/>
-      <c r="T40" s="92"/>
+      <c r="R40" s="92"/>
+      <c r="S40" s="92"/>
+      <c r="T40" s="93"/>
       <c r="U40" s="14"/>
       <c r="V40" s="14"/>
       <c r="W40" s="14"/>
       <c r="X40" s="15"/>
       <c r="Y40" s="22"/>
       <c r="Z40" s="23"/>
-      <c r="AA40" s="23"/>
+      <c r="AA40" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="AB40" s="23"/>
       <c r="AC40" s="24"/>
     </row>
@@ -2766,16 +2770,16 @@
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="48" t="s">
+      <c r="G41" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
       <c r="O41" s="13"/>
       <c r="P41" s="14"/>
       <c r="Q41" s="85" t="s">
@@ -2803,30 +2807,32 @@
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="48" t="s">
+      <c r="G42" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
       <c r="O42" s="13"/>
       <c r="P42" s="14"/>
-      <c r="Q42" s="93" t="s">
+      <c r="Q42" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R42" s="91"/>
-      <c r="S42" s="91"/>
-      <c r="T42" s="92"/>
+      <c r="R42" s="92"/>
+      <c r="S42" s="92"/>
+      <c r="T42" s="93"/>
       <c r="U42" s="14"/>
       <c r="V42" s="14"/>
       <c r="W42" s="14"/>
       <c r="X42" s="15"/>
       <c r="Y42" s="22"/>
-      <c r="Z42" s="23"/>
+      <c r="Z42" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="AA42" s="23"/>
       <c r="AB42" s="23"/>
       <c r="AC42" s="24"/>
@@ -2865,24 +2871,24 @@
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
       <c r="O44" s="13"/>
       <c r="P44" s="14"/>
-      <c r="Q44" s="93" t="s">
+      <c r="Q44" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R44" s="91"/>
-      <c r="S44" s="91"/>
-      <c r="T44" s="92"/>
+      <c r="R44" s="92"/>
+      <c r="S44" s="92"/>
+      <c r="T44" s="93"/>
       <c r="U44" s="17"/>
       <c r="V44" s="14"/>
       <c r="W44" s="14"/>
@@ -2910,12 +2916,12 @@
       <c r="N45" s="4"/>
       <c r="O45" s="13"/>
       <c r="P45" s="14"/>
-      <c r="Q45" s="93" t="s">
+      <c r="Q45" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R45" s="91"/>
-      <c r="S45" s="91"/>
-      <c r="T45" s="92"/>
+      <c r="R45" s="92"/>
+      <c r="S45" s="92"/>
+      <c r="T45" s="93"/>
       <c r="U45" s="17"/>
       <c r="V45" s="14"/>
       <c r="W45" s="14"/>
@@ -2931,24 +2937,24 @@
       <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="48" t="s">
+      <c r="G46" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
       <c r="O46" s="13"/>
       <c r="P46" s="14"/>
-      <c r="Q46" s="93" t="s">
+      <c r="Q46" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R46" s="91"/>
-      <c r="S46" s="91"/>
-      <c r="T46" s="92"/>
+      <c r="R46" s="92"/>
+      <c r="S46" s="92"/>
+      <c r="T46" s="93"/>
       <c r="U46" s="17"/>
       <c r="V46" s="14"/>
       <c r="W46" s="14"/>
@@ -2964,24 +2970,24 @@
       <c r="D47" s="4"/>
       <c r="E47" s="5"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="48" t="s">
+      <c r="G47" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
       <c r="O47" s="13"/>
       <c r="P47" s="14"/>
-      <c r="Q47" s="93" t="s">
+      <c r="Q47" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R47" s="91"/>
-      <c r="S47" s="91"/>
-      <c r="T47" s="92"/>
+      <c r="R47" s="92"/>
+      <c r="S47" s="92"/>
+      <c r="T47" s="93"/>
       <c r="U47" s="17"/>
       <c r="V47" s="14"/>
       <c r="W47" s="14"/>
@@ -3009,12 +3015,12 @@
       <c r="N48" s="4"/>
       <c r="O48" s="13"/>
       <c r="P48" s="14"/>
-      <c r="Q48" s="93" t="s">
+      <c r="Q48" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R48" s="91"/>
-      <c r="S48" s="91"/>
-      <c r="T48" s="92"/>
+      <c r="R48" s="92"/>
+      <c r="S48" s="92"/>
+      <c r="T48" s="93"/>
       <c r="U48" s="17"/>
       <c r="V48" s="14"/>
       <c r="W48" s="14"/>
@@ -3042,12 +3048,12 @@
       <c r="N49" s="4"/>
       <c r="O49" s="13"/>
       <c r="P49" s="14"/>
-      <c r="Q49" s="93" t="s">
+      <c r="Q49" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="R49" s="91"/>
-      <c r="S49" s="91"/>
-      <c r="T49" s="92"/>
+      <c r="R49" s="92"/>
+      <c r="S49" s="92"/>
+      <c r="T49" s="93"/>
       <c r="U49" s="17"/>
       <c r="V49" s="14"/>
       <c r="W49" s="14"/>
@@ -3104,7 +3110,7 @@
       <c r="N51" s="4"/>
       <c r="O51" s="13"/>
       <c r="P51" s="14"/>
-      <c r="Q51" s="80" t="s">
+      <c r="Q51" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R51" s="12"/>
@@ -3137,7 +3143,7 @@
       <c r="N52" s="4"/>
       <c r="O52" s="13"/>
       <c r="P52" s="14"/>
-      <c r="Q52" s="80" t="s">
+      <c r="Q52" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R52" s="12"/>
@@ -3170,7 +3176,7 @@
       <c r="N53" s="4"/>
       <c r="O53" s="13"/>
       <c r="P53" s="14"/>
-      <c r="Q53" s="80" t="s">
+      <c r="Q53" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R53" s="12"/>
@@ -3203,7 +3209,7 @@
       <c r="N54" s="4"/>
       <c r="O54" s="13"/>
       <c r="P54" s="14"/>
-      <c r="Q54" s="80" t="s">
+      <c r="Q54" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R54" s="12"/>
@@ -3236,7 +3242,7 @@
       <c r="N55" s="4"/>
       <c r="O55" s="13"/>
       <c r="P55" s="14"/>
-      <c r="Q55" s="80" t="s">
+      <c r="Q55" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R55" s="12"/>
@@ -3269,7 +3275,7 @@
       <c r="N56" s="4"/>
       <c r="O56" s="13"/>
       <c r="P56" s="14"/>
-      <c r="Q56" s="80" t="s">
+      <c r="Q56" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R56" s="12"/>
@@ -3302,7 +3308,7 @@
       <c r="N57" s="4"/>
       <c r="O57" s="13"/>
       <c r="P57" s="14"/>
-      <c r="Q57" s="80" t="s">
+      <c r="Q57" s="33" t="s">
         <v>70</v>
       </c>
       <c r="R57" s="12"/>
@@ -3521,7 +3527,7 @@
       <c r="N64" s="4"/>
       <c r="O64" s="13"/>
       <c r="P64" s="14"/>
-      <c r="Q64" s="79" t="s">
+      <c r="Q64" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R64" s="14"/>
@@ -3558,7 +3564,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="13"/>
       <c r="P65" s="14"/>
-      <c r="Q65" s="79" t="s">
+      <c r="Q65" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R65" s="14"/>
@@ -3734,206 +3740,206 @@
       </c>
     </row>
     <row r="71" spans="3:29">
-      <c r="C71" s="49" t="s">
+      <c r="C71" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D71" s="52" t="s">
+      <c r="D71" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="E71" s="55" t="s">
+      <c r="E71" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="F71" s="64"/>
-      <c r="G71" s="65"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="65"/>
-      <c r="J71" s="65"/>
-      <c r="K71" s="65"/>
-      <c r="L71" s="65"/>
-      <c r="M71" s="65"/>
-      <c r="N71" s="65"/>
-      <c r="O71" s="58">
+      <c r="F71" s="46"/>
+      <c r="G71" s="47"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="47"/>
+      <c r="M71" s="47"/>
+      <c r="N71" s="47"/>
+      <c r="O71" s="66">
         <v>43969</v>
       </c>
-      <c r="P71" s="60">
+      <c r="P71" s="68">
         <v>43976</v>
       </c>
-      <c r="Q71" s="60">
+      <c r="Q71" s="68">
         <v>43983</v>
       </c>
-      <c r="R71" s="60">
+      <c r="R71" s="68">
         <v>43990</v>
       </c>
-      <c r="S71" s="60">
+      <c r="S71" s="68">
         <v>43997</v>
       </c>
-      <c r="T71" s="60">
+      <c r="T71" s="68">
         <v>44004</v>
       </c>
-      <c r="U71" s="60">
+      <c r="U71" s="68">
         <v>44011</v>
       </c>
-      <c r="V71" s="60">
+      <c r="V71" s="68">
         <v>44018</v>
       </c>
-      <c r="W71" s="60">
+      <c r="W71" s="68">
         <v>44025</v>
       </c>
-      <c r="X71" s="62">
+      <c r="X71" s="70">
         <v>44032</v>
       </c>
-      <c r="Y71" s="70" t="s">
+      <c r="Y71" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="Z71" s="71"/>
-      <c r="AA71" s="71"/>
-      <c r="AB71" s="71"/>
-      <c r="AC71" s="72"/>
+      <c r="Z71" s="73"/>
+      <c r="AA71" s="73"/>
+      <c r="AB71" s="73"/>
+      <c r="AC71" s="74"/>
     </row>
     <row r="72" spans="3:29">
-      <c r="C72" s="50"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="78"/>
-      <c r="I72" s="78"/>
-      <c r="J72" s="78"/>
-      <c r="K72" s="78"/>
-      <c r="L72" s="78"/>
-      <c r="M72" s="78"/>
-      <c r="N72" s="78"/>
-      <c r="O72" s="58"/>
-      <c r="P72" s="60"/>
-      <c r="Q72" s="60"/>
-      <c r="R72" s="60"/>
-      <c r="S72" s="60"/>
-      <c r="T72" s="60"/>
-      <c r="U72" s="60"/>
-      <c r="V72" s="60"/>
-      <c r="W72" s="60"/>
-      <c r="X72" s="62"/>
-      <c r="Y72" s="73"/>
-      <c r="Z72" s="71"/>
-      <c r="AA72" s="71"/>
-      <c r="AB72" s="71"/>
-      <c r="AC72" s="72"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="80"/>
+      <c r="K72" s="80"/>
+      <c r="L72" s="80"/>
+      <c r="M72" s="80"/>
+      <c r="N72" s="80"/>
+      <c r="O72" s="66"/>
+      <c r="P72" s="68"/>
+      <c r="Q72" s="68"/>
+      <c r="R72" s="68"/>
+      <c r="S72" s="68"/>
+      <c r="T72" s="68"/>
+      <c r="U72" s="68"/>
+      <c r="V72" s="68"/>
+      <c r="W72" s="68"/>
+      <c r="X72" s="70"/>
+      <c r="Y72" s="75"/>
+      <c r="Z72" s="73"/>
+      <c r="AA72" s="73"/>
+      <c r="AB72" s="73"/>
+      <c r="AC72" s="74"/>
     </row>
     <row r="73" spans="3:29">
-      <c r="C73" s="50"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="77"/>
-      <c r="G73" s="78"/>
-      <c r="H73" s="78"/>
-      <c r="I73" s="78"/>
-      <c r="J73" s="78"/>
-      <c r="K73" s="78"/>
-      <c r="L73" s="78"/>
-      <c r="M73" s="78"/>
-      <c r="N73" s="78"/>
-      <c r="O73" s="58"/>
-      <c r="P73" s="60"/>
-      <c r="Q73" s="60"/>
-      <c r="R73" s="60"/>
-      <c r="S73" s="60"/>
-      <c r="T73" s="60"/>
-      <c r="U73" s="60"/>
-      <c r="V73" s="60"/>
-      <c r="W73" s="60"/>
-      <c r="X73" s="62"/>
-      <c r="Y73" s="73"/>
-      <c r="Z73" s="71"/>
-      <c r="AA73" s="71"/>
-      <c r="AB73" s="71"/>
-      <c r="AC73" s="72"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="79"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="80"/>
+      <c r="I73" s="80"/>
+      <c r="J73" s="80"/>
+      <c r="K73" s="80"/>
+      <c r="L73" s="80"/>
+      <c r="M73" s="80"/>
+      <c r="N73" s="80"/>
+      <c r="O73" s="66"/>
+      <c r="P73" s="68"/>
+      <c r="Q73" s="68"/>
+      <c r="R73" s="68"/>
+      <c r="S73" s="68"/>
+      <c r="T73" s="68"/>
+      <c r="U73" s="68"/>
+      <c r="V73" s="68"/>
+      <c r="W73" s="68"/>
+      <c r="X73" s="70"/>
+      <c r="Y73" s="75"/>
+      <c r="Z73" s="73"/>
+      <c r="AA73" s="73"/>
+      <c r="AB73" s="73"/>
+      <c r="AC73" s="74"/>
     </row>
     <row r="74" spans="3:29">
-      <c r="C74" s="50"/>
-      <c r="D74" s="53"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="77"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="78"/>
-      <c r="J74" s="78"/>
-      <c r="K74" s="78"/>
-      <c r="L74" s="78"/>
-      <c r="M74" s="78"/>
-      <c r="N74" s="78"/>
-      <c r="O74" s="58"/>
-      <c r="P74" s="60"/>
-      <c r="Q74" s="60"/>
-      <c r="R74" s="60"/>
-      <c r="S74" s="60"/>
-      <c r="T74" s="60"/>
-      <c r="U74" s="60"/>
-      <c r="V74" s="60"/>
-      <c r="W74" s="60"/>
-      <c r="X74" s="62"/>
-      <c r="Y74" s="73"/>
-      <c r="Z74" s="71"/>
-      <c r="AA74" s="71"/>
-      <c r="AB74" s="71"/>
-      <c r="AC74" s="72"/>
+      <c r="C74" s="58"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="80"/>
+      <c r="H74" s="80"/>
+      <c r="I74" s="80"/>
+      <c r="J74" s="80"/>
+      <c r="K74" s="80"/>
+      <c r="L74" s="80"/>
+      <c r="M74" s="80"/>
+      <c r="N74" s="80"/>
+      <c r="O74" s="66"/>
+      <c r="P74" s="68"/>
+      <c r="Q74" s="68"/>
+      <c r="R74" s="68"/>
+      <c r="S74" s="68"/>
+      <c r="T74" s="68"/>
+      <c r="U74" s="68"/>
+      <c r="V74" s="68"/>
+      <c r="W74" s="68"/>
+      <c r="X74" s="70"/>
+      <c r="Y74" s="75"/>
+      <c r="Z74" s="73"/>
+      <c r="AA74" s="73"/>
+      <c r="AB74" s="73"/>
+      <c r="AC74" s="74"/>
     </row>
     <row r="75" spans="3:29">
-      <c r="C75" s="50"/>
-      <c r="D75" s="53"/>
-      <c r="E75" s="56"/>
-      <c r="F75" s="77"/>
-      <c r="G75" s="78"/>
-      <c r="H75" s="78"/>
-      <c r="I75" s="78"/>
-      <c r="J75" s="78"/>
-      <c r="K75" s="78"/>
-      <c r="L75" s="78"/>
-      <c r="M75" s="78"/>
-      <c r="N75" s="78"/>
-      <c r="O75" s="58"/>
-      <c r="P75" s="60"/>
-      <c r="Q75" s="60"/>
-      <c r="R75" s="60"/>
-      <c r="S75" s="60"/>
-      <c r="T75" s="60"/>
-      <c r="U75" s="60"/>
-      <c r="V75" s="60"/>
-      <c r="W75" s="60"/>
-      <c r="X75" s="62"/>
-      <c r="Y75" s="73"/>
-      <c r="Z75" s="71"/>
-      <c r="AA75" s="71"/>
-      <c r="AB75" s="71"/>
-      <c r="AC75" s="72"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="79"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="80"/>
+      <c r="I75" s="80"/>
+      <c r="J75" s="80"/>
+      <c r="K75" s="80"/>
+      <c r="L75" s="80"/>
+      <c r="M75" s="80"/>
+      <c r="N75" s="80"/>
+      <c r="O75" s="66"/>
+      <c r="P75" s="68"/>
+      <c r="Q75" s="68"/>
+      <c r="R75" s="68"/>
+      <c r="S75" s="68"/>
+      <c r="T75" s="68"/>
+      <c r="U75" s="68"/>
+      <c r="V75" s="68"/>
+      <c r="W75" s="68"/>
+      <c r="X75" s="70"/>
+      <c r="Y75" s="75"/>
+      <c r="Z75" s="73"/>
+      <c r="AA75" s="73"/>
+      <c r="AB75" s="73"/>
+      <c r="AC75" s="74"/>
     </row>
     <row r="76" spans="3:29">
-      <c r="C76" s="51"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="57"/>
-      <c r="F76" s="67"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="68"/>
-      <c r="J76" s="68"/>
-      <c r="K76" s="68"/>
-      <c r="L76" s="68"/>
-      <c r="M76" s="68"/>
-      <c r="N76" s="68"/>
-      <c r="O76" s="59"/>
-      <c r="P76" s="61"/>
-      <c r="Q76" s="61"/>
-      <c r="R76" s="61"/>
-      <c r="S76" s="61"/>
-      <c r="T76" s="61"/>
-      <c r="U76" s="61"/>
-      <c r="V76" s="61"/>
-      <c r="W76" s="61"/>
-      <c r="X76" s="63"/>
-      <c r="Y76" s="74"/>
-      <c r="Z76" s="75"/>
-      <c r="AA76" s="75"/>
-      <c r="AB76" s="75"/>
-      <c r="AC76" s="76"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="62"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="50"/>
+      <c r="H76" s="50"/>
+      <c r="I76" s="50"/>
+      <c r="J76" s="50"/>
+      <c r="K76" s="50"/>
+      <c r="L76" s="50"/>
+      <c r="M76" s="50"/>
+      <c r="N76" s="50"/>
+      <c r="O76" s="67"/>
+      <c r="P76" s="69"/>
+      <c r="Q76" s="69"/>
+      <c r="R76" s="69"/>
+      <c r="S76" s="69"/>
+      <c r="T76" s="69"/>
+      <c r="U76" s="69"/>
+      <c r="V76" s="69"/>
+      <c r="W76" s="69"/>
+      <c r="X76" s="71"/>
+      <c r="Y76" s="76"/>
+      <c r="Z76" s="77"/>
+      <c r="AA76" s="77"/>
+      <c r="AB76" s="77"/>
+      <c r="AC76" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="77">

</xml_diff>

<commit_message>
[document] update srs & plan
</commit_message>
<xml_diff>
--- a/document/Plan.xlsx
+++ b/document/Plan.xlsx
@@ -658,6 +658,138 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -682,143 +814,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1363,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1383,107 +1383,107 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:29">
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="35" t="s">
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="81"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="35" t="s">
+      <c r="AB2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="36"/>
+      <c r="AC2" s="82"/>
     </row>
     <row r="3" spans="3:29">
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="38"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="84"/>
     </row>
     <row r="4" spans="3:29">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42" t="s">
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="43" t="s">
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="39" t="s">
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="41"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
     </row>
     <row r="5" spans="3:29">
       <c r="C5" s="3"/>
@@ -1646,10 +1646,10 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="81" t="s">
+      <c r="O9" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="P9" s="82"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
@@ -1690,10 +1690,10 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="13"/>
-      <c r="P10" s="81" t="s">
+      <c r="P10" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q10" s="82"/>
+      <c r="Q10" s="59"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
@@ -1762,10 +1762,10 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="83" t="s">
+      <c r="P12" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="84"/>
+      <c r="Q12" s="35"/>
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
@@ -1801,10 +1801,10 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="13"/>
-      <c r="P13" s="81" t="s">
+      <c r="P13" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q13" s="82"/>
+      <c r="Q13" s="59"/>
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
@@ -1840,10 +1840,10 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="13"/>
-      <c r="P14" s="81" t="s">
+      <c r="P14" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q14" s="82"/>
+      <c r="Q14" s="59"/>
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
@@ -1877,10 +1877,10 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="13"/>
-      <c r="P15" s="81" t="s">
+      <c r="P15" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q15" s="82"/>
+      <c r="Q15" s="59"/>
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
@@ -1916,10 +1916,10 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="81" t="s">
+      <c r="P16" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="Q16" s="82"/>
+      <c r="Q16" s="59"/>
       <c r="R16" s="14"/>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -1955,10 +1955,10 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="13"/>
-      <c r="P17" s="83" t="s">
+      <c r="P17" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="Q17" s="84"/>
+      <c r="Q17" s="35"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
@@ -2012,16 +2012,16 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
       <c r="O19" s="13"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="32" t="s">
@@ -2049,19 +2049,19 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="53" t="s">
+      <c r="G20" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
       <c r="O20" s="13"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="33" t="s">
+      <c r="Q20" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R20" s="14"/>
@@ -2086,19 +2086,19 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="53" t="s">
+      <c r="G21" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
       <c r="O21" s="13"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="32" t="s">
         <v>70</v>
       </c>
       <c r="R21" s="14"/>
@@ -2123,16 +2123,16 @@
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
       <c r="O22" s="13"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="32" t="s">
@@ -2189,22 +2189,22 @@
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="54" t="s">
+      <c r="G24" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
       <c r="O24" s="13"/>
       <c r="P24" s="14"/>
-      <c r="Q24" s="81" t="s">
+      <c r="Q24" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="R24" s="82"/>
+      <c r="R24" s="59"/>
       <c r="S24" s="14"/>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
@@ -2224,22 +2224,22 @@
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="54" t="s">
+      <c r="G25" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
       <c r="O25" s="13"/>
       <c r="P25" s="14"/>
-      <c r="Q25" s="81" t="s">
+      <c r="Q25" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="R25" s="82"/>
+      <c r="R25" s="59"/>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
       <c r="U25" s="14"/>
@@ -2259,22 +2259,22 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
       <c r="O26" s="13"/>
       <c r="P26" s="14"/>
-      <c r="Q26" s="81" t="s">
+      <c r="Q26" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="R26" s="82"/>
+      <c r="R26" s="59"/>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
       <c r="U26" s="14"/>
@@ -2296,22 +2296,22 @@
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="54" t="s">
+      <c r="G27" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
       <c r="O27" s="13"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="81" t="s">
+      <c r="Q27" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="R27" s="82"/>
+      <c r="R27" s="59"/>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
       <c r="U27" s="14"/>
@@ -2362,23 +2362,23 @@
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="54" t="s">
+      <c r="G29" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
       <c r="O29" s="13"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
-      <c r="R29" s="85" t="s">
+      <c r="R29" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="S29" s="86"/>
+      <c r="S29" s="41"/>
       <c r="T29" s="14"/>
       <c r="U29" s="14"/>
       <c r="V29" s="14"/>
@@ -2399,23 +2399,23 @@
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="54" t="s">
+      <c r="G30" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
       <c r="O30" s="13"/>
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
-      <c r="R30" s="85" t="s">
+      <c r="R30" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="S30" s="86"/>
+      <c r="S30" s="41"/>
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
       <c r="V30" s="14"/>
@@ -2436,23 +2436,23 @@
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="55" t="s">
+      <c r="G31" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
       <c r="O31" s="13"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
-      <c r="R31" s="85" t="s">
+      <c r="R31" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="S31" s="86"/>
+      <c r="S31" s="41"/>
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
@@ -2469,23 +2469,23 @@
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="54" t="s">
+      <c r="G32" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
       <c r="O32" s="13"/>
       <c r="P32" s="14"/>
       <c r="Q32" s="14"/>
-      <c r="R32" s="83" t="s">
+      <c r="R32" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="S32" s="84"/>
+      <c r="S32" s="41"/>
       <c r="T32" s="14"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
@@ -2562,23 +2562,23 @@
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
       <c r="O35" s="13"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="87" t="s">
+      <c r="Q35" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="R35" s="88"/>
-      <c r="S35" s="89"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="44"/>
       <c r="T35" s="14"/>
       <c r="U35" s="14"/>
       <c r="V35" s="14"/>
@@ -2624,24 +2624,24 @@
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="53" t="s">
+      <c r="G37" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
       <c r="O37" s="13"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="85" t="s">
+      <c r="Q37" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="R37" s="90"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="86"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="41"/>
       <c r="U37" s="14"/>
       <c r="V37" s="14"/>
       <c r="W37" s="14"/>
@@ -2661,24 +2661,24 @@
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="56" t="s">
+      <c r="G38" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="76"/>
       <c r="O38" s="13"/>
       <c r="P38" s="14"/>
-      <c r="Q38" s="85" t="s">
+      <c r="Q38" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="R38" s="90"/>
-      <c r="S38" s="90"/>
-      <c r="T38" s="86"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="40"/>
+      <c r="T38" s="41"/>
       <c r="U38" s="14"/>
       <c r="V38" s="14"/>
       <c r="W38" s="14"/>
@@ -2698,24 +2698,24 @@
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="56" t="s">
+      <c r="G39" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="76"/>
+      <c r="N39" s="76"/>
       <c r="O39" s="13"/>
       <c r="P39" s="14"/>
-      <c r="Q39" s="85" t="s">
+      <c r="Q39" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="R39" s="90"/>
-      <c r="S39" s="90"/>
-      <c r="T39" s="86"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="41"/>
       <c r="U39" s="14"/>
       <c r="V39" s="14"/>
       <c r="W39" s="14"/>
@@ -2735,24 +2735,24 @@
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
       <c r="O40" s="13"/>
       <c r="P40" s="14"/>
-      <c r="Q40" s="91" t="s">
+      <c r="Q40" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R40" s="92"/>
-      <c r="S40" s="92"/>
-      <c r="T40" s="93"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="38"/>
       <c r="U40" s="14"/>
       <c r="V40" s="14"/>
       <c r="W40" s="14"/>
@@ -2770,24 +2770,24 @@
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="56" t="s">
+      <c r="G41" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="66"/>
       <c r="O41" s="13"/>
       <c r="P41" s="14"/>
-      <c r="Q41" s="85" t="s">
+      <c r="Q41" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
-      <c r="T41" s="86"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="41"/>
       <c r="U41" s="14"/>
       <c r="V41" s="14"/>
       <c r="W41" s="14"/>
@@ -2807,24 +2807,24 @@
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="56" t="s">
+      <c r="G42" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="66"/>
+      <c r="N42" s="66"/>
       <c r="O42" s="13"/>
       <c r="P42" s="14"/>
-      <c r="Q42" s="91" t="s">
+      <c r="Q42" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="R42" s="92"/>
-      <c r="S42" s="92"/>
-      <c r="T42" s="93"/>
+      <c r="R42" s="40"/>
+      <c r="S42" s="40"/>
+      <c r="T42" s="41"/>
       <c r="U42" s="14"/>
       <c r="V42" s="14"/>
       <c r="W42" s="14"/>
@@ -2871,24 +2871,24 @@
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="56" t="s">
+      <c r="G44" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="66"/>
       <c r="O44" s="13"/>
       <c r="P44" s="14"/>
-      <c r="Q44" s="91" t="s">
+      <c r="Q44" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R44" s="92"/>
-      <c r="S44" s="92"/>
-      <c r="T44" s="93"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="38"/>
       <c r="U44" s="17"/>
       <c r="V44" s="14"/>
       <c r="W44" s="14"/>
@@ -2916,12 +2916,12 @@
       <c r="N45" s="4"/>
       <c r="O45" s="13"/>
       <c r="P45" s="14"/>
-      <c r="Q45" s="91" t="s">
+      <c r="Q45" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R45" s="92"/>
-      <c r="S45" s="92"/>
-      <c r="T45" s="93"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="38"/>
       <c r="U45" s="17"/>
       <c r="V45" s="14"/>
       <c r="W45" s="14"/>
@@ -2937,24 +2937,24 @@
       <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="56" t="s">
+      <c r="G46" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="66"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="66"/>
       <c r="O46" s="13"/>
       <c r="P46" s="14"/>
-      <c r="Q46" s="91" t="s">
+      <c r="Q46" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R46" s="92"/>
-      <c r="S46" s="92"/>
-      <c r="T46" s="93"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="38"/>
       <c r="U46" s="17"/>
       <c r="V46" s="14"/>
       <c r="W46" s="14"/>
@@ -2970,24 +2970,24 @@
       <c r="D47" s="4"/>
       <c r="E47" s="5"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="56" t="s">
+      <c r="G47" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
+      <c r="L47" s="66"/>
+      <c r="M47" s="66"/>
+      <c r="N47" s="66"/>
       <c r="O47" s="13"/>
       <c r="P47" s="14"/>
-      <c r="Q47" s="91" t="s">
+      <c r="Q47" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R47" s="92"/>
-      <c r="S47" s="92"/>
-      <c r="T47" s="93"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="38"/>
       <c r="U47" s="17"/>
       <c r="V47" s="14"/>
       <c r="W47" s="14"/>
@@ -3015,12 +3015,12 @@
       <c r="N48" s="4"/>
       <c r="O48" s="13"/>
       <c r="P48" s="14"/>
-      <c r="Q48" s="91" t="s">
+      <c r="Q48" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R48" s="92"/>
-      <c r="S48" s="92"/>
-      <c r="T48" s="93"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="38"/>
       <c r="U48" s="17"/>
       <c r="V48" s="14"/>
       <c r="W48" s="14"/>
@@ -3048,12 +3048,12 @@
       <c r="N49" s="4"/>
       <c r="O49" s="13"/>
       <c r="P49" s="14"/>
-      <c r="Q49" s="91" t="s">
+      <c r="Q49" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R49" s="92"/>
-      <c r="S49" s="92"/>
-      <c r="T49" s="93"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="38"/>
       <c r="U49" s="17"/>
       <c r="V49" s="14"/>
       <c r="W49" s="14"/>
@@ -3432,10 +3432,10 @@
       <c r="N61" s="4"/>
       <c r="O61" s="13"/>
       <c r="P61" s="14"/>
-      <c r="Q61" s="83" t="s">
+      <c r="Q61" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="R61" s="84"/>
+      <c r="R61" s="35"/>
       <c r="S61" s="12"/>
       <c r="T61" s="12"/>
       <c r="U61" s="12"/>
@@ -3467,10 +3467,10 @@
       <c r="P62" s="14"/>
       <c r="Q62" s="14"/>
       <c r="R62" s="12"/>
-      <c r="S62" s="83" t="s">
+      <c r="S62" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="T62" s="84"/>
+      <c r="T62" s="35"/>
       <c r="U62" s="17"/>
       <c r="V62" s="17"/>
       <c r="W62" s="14"/>
@@ -3740,226 +3740,253 @@
       </c>
     </row>
     <row r="71" spans="3:29">
-      <c r="C71" s="57" t="s">
+      <c r="C71" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="D71" s="60" t="s">
+      <c r="D71" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="E71" s="63" t="s">
+      <c r="E71" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="F71" s="46"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="47"/>
-      <c r="L71" s="47"/>
-      <c r="M71" s="47"/>
-      <c r="N71" s="47"/>
-      <c r="O71" s="66">
+      <c r="F71" s="52"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
+      <c r="L71" s="53"/>
+      <c r="M71" s="53"/>
+      <c r="N71" s="53"/>
+      <c r="O71" s="64">
         <v>43969</v>
       </c>
-      <c r="P71" s="68">
+      <c r="P71" s="60">
         <v>43976</v>
       </c>
-      <c r="Q71" s="68">
+      <c r="Q71" s="60">
         <v>43983</v>
       </c>
-      <c r="R71" s="68">
+      <c r="R71" s="60">
         <v>43990</v>
       </c>
-      <c r="S71" s="68">
+      <c r="S71" s="60">
         <v>43997</v>
       </c>
-      <c r="T71" s="68">
+      <c r="T71" s="60">
         <v>44004</v>
       </c>
-      <c r="U71" s="68">
+      <c r="U71" s="60">
         <v>44011</v>
       </c>
-      <c r="V71" s="68">
+      <c r="V71" s="60">
         <v>44018</v>
       </c>
-      <c r="W71" s="68">
+      <c r="W71" s="60">
         <v>44025</v>
       </c>
-      <c r="X71" s="70">
+      <c r="X71" s="62">
         <v>44032</v>
       </c>
-      <c r="Y71" s="72" t="s">
+      <c r="Y71" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="Z71" s="73"/>
-      <c r="AA71" s="73"/>
-      <c r="AB71" s="73"/>
-      <c r="AC71" s="74"/>
+      <c r="Z71" s="46"/>
+      <c r="AA71" s="46"/>
+      <c r="AB71" s="46"/>
+      <c r="AC71" s="47"/>
     </row>
     <row r="72" spans="3:29">
-      <c r="C72" s="58"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="79"/>
-      <c r="G72" s="80"/>
-      <c r="H72" s="80"/>
-      <c r="I72" s="80"/>
-      <c r="J72" s="80"/>
-      <c r="K72" s="80"/>
-      <c r="L72" s="80"/>
-      <c r="M72" s="80"/>
-      <c r="N72" s="80"/>
-      <c r="O72" s="66"/>
-      <c r="P72" s="68"/>
-      <c r="Q72" s="68"/>
-      <c r="R72" s="68"/>
-      <c r="S72" s="68"/>
-      <c r="T72" s="68"/>
-      <c r="U72" s="68"/>
-      <c r="V72" s="68"/>
-      <c r="W72" s="68"/>
-      <c r="X72" s="70"/>
-      <c r="Y72" s="75"/>
-      <c r="Z72" s="73"/>
-      <c r="AA72" s="73"/>
-      <c r="AB72" s="73"/>
-      <c r="AC72" s="74"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="55"/>
+      <c r="I72" s="55"/>
+      <c r="J72" s="55"/>
+      <c r="K72" s="55"/>
+      <c r="L72" s="55"/>
+      <c r="M72" s="55"/>
+      <c r="N72" s="55"/>
+      <c r="O72" s="64"/>
+      <c r="P72" s="60"/>
+      <c r="Q72" s="60"/>
+      <c r="R72" s="60"/>
+      <c r="S72" s="60"/>
+      <c r="T72" s="60"/>
+      <c r="U72" s="60"/>
+      <c r="V72" s="60"/>
+      <c r="W72" s="60"/>
+      <c r="X72" s="62"/>
+      <c r="Y72" s="48"/>
+      <c r="Z72" s="46"/>
+      <c r="AA72" s="46"/>
+      <c r="AB72" s="46"/>
+      <c r="AC72" s="47"/>
     </row>
     <row r="73" spans="3:29">
-      <c r="C73" s="58"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="79"/>
-      <c r="G73" s="80"/>
-      <c r="H73" s="80"/>
-      <c r="I73" s="80"/>
-      <c r="J73" s="80"/>
-      <c r="K73" s="80"/>
-      <c r="L73" s="80"/>
-      <c r="M73" s="80"/>
-      <c r="N73" s="80"/>
-      <c r="O73" s="66"/>
-      <c r="P73" s="68"/>
-      <c r="Q73" s="68"/>
-      <c r="R73" s="68"/>
-      <c r="S73" s="68"/>
-      <c r="T73" s="68"/>
-      <c r="U73" s="68"/>
-      <c r="V73" s="68"/>
-      <c r="W73" s="68"/>
-      <c r="X73" s="70"/>
-      <c r="Y73" s="75"/>
-      <c r="Z73" s="73"/>
-      <c r="AA73" s="73"/>
-      <c r="AB73" s="73"/>
-      <c r="AC73" s="74"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="55"/>
+      <c r="I73" s="55"/>
+      <c r="J73" s="55"/>
+      <c r="K73" s="55"/>
+      <c r="L73" s="55"/>
+      <c r="M73" s="55"/>
+      <c r="N73" s="55"/>
+      <c r="O73" s="64"/>
+      <c r="P73" s="60"/>
+      <c r="Q73" s="60"/>
+      <c r="R73" s="60"/>
+      <c r="S73" s="60"/>
+      <c r="T73" s="60"/>
+      <c r="U73" s="60"/>
+      <c r="V73" s="60"/>
+      <c r="W73" s="60"/>
+      <c r="X73" s="62"/>
+      <c r="Y73" s="48"/>
+      <c r="Z73" s="46"/>
+      <c r="AA73" s="46"/>
+      <c r="AB73" s="46"/>
+      <c r="AC73" s="47"/>
     </row>
     <row r="74" spans="3:29">
-      <c r="C74" s="58"/>
-      <c r="D74" s="61"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="79"/>
-      <c r="G74" s="80"/>
-      <c r="H74" s="80"/>
-      <c r="I74" s="80"/>
-      <c r="J74" s="80"/>
-      <c r="K74" s="80"/>
-      <c r="L74" s="80"/>
-      <c r="M74" s="80"/>
-      <c r="N74" s="80"/>
-      <c r="O74" s="66"/>
-      <c r="P74" s="68"/>
-      <c r="Q74" s="68"/>
-      <c r="R74" s="68"/>
-      <c r="S74" s="68"/>
-      <c r="T74" s="68"/>
-      <c r="U74" s="68"/>
-      <c r="V74" s="68"/>
-      <c r="W74" s="68"/>
-      <c r="X74" s="70"/>
-      <c r="Y74" s="75"/>
-      <c r="Z74" s="73"/>
-      <c r="AA74" s="73"/>
-      <c r="AB74" s="73"/>
-      <c r="AC74" s="74"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="54"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="55"/>
+      <c r="I74" s="55"/>
+      <c r="J74" s="55"/>
+      <c r="K74" s="55"/>
+      <c r="L74" s="55"/>
+      <c r="M74" s="55"/>
+      <c r="N74" s="55"/>
+      <c r="O74" s="64"/>
+      <c r="P74" s="60"/>
+      <c r="Q74" s="60"/>
+      <c r="R74" s="60"/>
+      <c r="S74" s="60"/>
+      <c r="T74" s="60"/>
+      <c r="U74" s="60"/>
+      <c r="V74" s="60"/>
+      <c r="W74" s="60"/>
+      <c r="X74" s="62"/>
+      <c r="Y74" s="48"/>
+      <c r="Z74" s="46"/>
+      <c r="AA74" s="46"/>
+      <c r="AB74" s="46"/>
+      <c r="AC74" s="47"/>
     </row>
     <row r="75" spans="3:29">
-      <c r="C75" s="58"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="79"/>
-      <c r="G75" s="80"/>
-      <c r="H75" s="80"/>
-      <c r="I75" s="80"/>
-      <c r="J75" s="80"/>
-      <c r="K75" s="80"/>
-      <c r="L75" s="80"/>
-      <c r="M75" s="80"/>
-      <c r="N75" s="80"/>
-      <c r="O75" s="66"/>
-      <c r="P75" s="68"/>
-      <c r="Q75" s="68"/>
-      <c r="R75" s="68"/>
-      <c r="S75" s="68"/>
-      <c r="T75" s="68"/>
-      <c r="U75" s="68"/>
-      <c r="V75" s="68"/>
-      <c r="W75" s="68"/>
-      <c r="X75" s="70"/>
-      <c r="Y75" s="75"/>
-      <c r="Z75" s="73"/>
-      <c r="AA75" s="73"/>
-      <c r="AB75" s="73"/>
-      <c r="AC75" s="74"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
+      <c r="I75" s="55"/>
+      <c r="J75" s="55"/>
+      <c r="K75" s="55"/>
+      <c r="L75" s="55"/>
+      <c r="M75" s="55"/>
+      <c r="N75" s="55"/>
+      <c r="O75" s="64"/>
+      <c r="P75" s="60"/>
+      <c r="Q75" s="60"/>
+      <c r="R75" s="60"/>
+      <c r="S75" s="60"/>
+      <c r="T75" s="60"/>
+      <c r="U75" s="60"/>
+      <c r="V75" s="60"/>
+      <c r="W75" s="60"/>
+      <c r="X75" s="62"/>
+      <c r="Y75" s="48"/>
+      <c r="Z75" s="46"/>
+      <c r="AA75" s="46"/>
+      <c r="AB75" s="46"/>
+      <c r="AC75" s="47"/>
     </row>
     <row r="76" spans="3:29">
-      <c r="C76" s="59"/>
-      <c r="D76" s="62"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="50"/>
-      <c r="H76" s="50"/>
-      <c r="I76" s="50"/>
-      <c r="J76" s="50"/>
-      <c r="K76" s="50"/>
-      <c r="L76" s="50"/>
-      <c r="M76" s="50"/>
-      <c r="N76" s="50"/>
-      <c r="O76" s="67"/>
-      <c r="P76" s="69"/>
-      <c r="Q76" s="69"/>
-      <c r="R76" s="69"/>
-      <c r="S76" s="69"/>
-      <c r="T76" s="69"/>
-      <c r="U76" s="69"/>
-      <c r="V76" s="69"/>
-      <c r="W76" s="69"/>
-      <c r="X76" s="71"/>
-      <c r="Y76" s="76"/>
-      <c r="Z76" s="77"/>
-      <c r="AA76" s="77"/>
-      <c r="AB76" s="77"/>
-      <c r="AC76" s="78"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="72"/>
+      <c r="E76" s="75"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="57"/>
+      <c r="H76" s="57"/>
+      <c r="I76" s="57"/>
+      <c r="J76" s="57"/>
+      <c r="K76" s="57"/>
+      <c r="L76" s="57"/>
+      <c r="M76" s="57"/>
+      <c r="N76" s="57"/>
+      <c r="O76" s="65"/>
+      <c r="P76" s="61"/>
+      <c r="Q76" s="61"/>
+      <c r="R76" s="61"/>
+      <c r="S76" s="61"/>
+      <c r="T76" s="61"/>
+      <c r="U76" s="61"/>
+      <c r="V76" s="61"/>
+      <c r="W76" s="61"/>
+      <c r="X76" s="63"/>
+      <c r="Y76" s="49"/>
+      <c r="Z76" s="50"/>
+      <c r="AA76" s="50"/>
+      <c r="AB76" s="50"/>
+      <c r="AC76" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="Q45:T45"/>
-    <mergeCell ref="Q46:T46"/>
-    <mergeCell ref="Q47:T47"/>
-    <mergeCell ref="Q48:T48"/>
-    <mergeCell ref="Q49:T49"/>
-    <mergeCell ref="Q39:T39"/>
-    <mergeCell ref="Q41:T41"/>
-    <mergeCell ref="Q40:T40"/>
-    <mergeCell ref="Q42:T42"/>
-    <mergeCell ref="Q44:T44"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="Q37:T37"/>
-    <mergeCell ref="Q38:T38"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="O2:Z2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="F3:AC3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="O4:X4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="C2:E3"/>
+    <mergeCell ref="G19:N19"/>
+    <mergeCell ref="G20:N20"/>
+    <mergeCell ref="G21:N21"/>
+    <mergeCell ref="G22:N22"/>
+    <mergeCell ref="G24:N24"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="G26:N26"/>
+    <mergeCell ref="G27:N27"/>
+    <mergeCell ref="G29:N29"/>
+    <mergeCell ref="G30:N30"/>
+    <mergeCell ref="G31:N31"/>
+    <mergeCell ref="G32:N32"/>
+    <mergeCell ref="G35:N35"/>
+    <mergeCell ref="G37:N37"/>
+    <mergeCell ref="G38:N38"/>
+    <mergeCell ref="G39:N39"/>
+    <mergeCell ref="G40:N40"/>
+    <mergeCell ref="G41:N41"/>
+    <mergeCell ref="G42:N42"/>
+    <mergeCell ref="G44:N44"/>
+    <mergeCell ref="G46:N46"/>
+    <mergeCell ref="G47:N47"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="D71:D76"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="O71:O76"/>
+    <mergeCell ref="P71:P76"/>
+    <mergeCell ref="Q71:Q76"/>
+    <mergeCell ref="R71:R76"/>
+    <mergeCell ref="S71:S76"/>
+    <mergeCell ref="T71:T76"/>
+    <mergeCell ref="U71:U76"/>
+    <mergeCell ref="V71:V76"/>
+    <mergeCell ref="W71:W76"/>
+    <mergeCell ref="X71:X76"/>
     <mergeCell ref="Y71:AC76"/>
     <mergeCell ref="F71:N76"/>
     <mergeCell ref="O9:P9"/>
@@ -3976,50 +4003,23 @@
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="R29:S29"/>
     <mergeCell ref="R30:S30"/>
-    <mergeCell ref="T71:T76"/>
-    <mergeCell ref="U71:U76"/>
-    <mergeCell ref="V71:V76"/>
-    <mergeCell ref="W71:W76"/>
-    <mergeCell ref="X71:X76"/>
-    <mergeCell ref="O71:O76"/>
-    <mergeCell ref="P71:P76"/>
-    <mergeCell ref="Q71:Q76"/>
-    <mergeCell ref="R71:R76"/>
-    <mergeCell ref="S71:S76"/>
-    <mergeCell ref="G46:N46"/>
-    <mergeCell ref="G47:N47"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="D71:D76"/>
-    <mergeCell ref="E71:E76"/>
-    <mergeCell ref="G39:N39"/>
-    <mergeCell ref="G40:N40"/>
-    <mergeCell ref="G41:N41"/>
-    <mergeCell ref="G42:N42"/>
-    <mergeCell ref="G44:N44"/>
-    <mergeCell ref="G31:N31"/>
-    <mergeCell ref="G32:N32"/>
-    <mergeCell ref="G35:N35"/>
-    <mergeCell ref="G37:N37"/>
-    <mergeCell ref="G38:N38"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="G26:N26"/>
-    <mergeCell ref="G27:N27"/>
-    <mergeCell ref="G29:N29"/>
-    <mergeCell ref="G30:N30"/>
-    <mergeCell ref="G19:N19"/>
-    <mergeCell ref="G20:N20"/>
-    <mergeCell ref="G21:N21"/>
-    <mergeCell ref="G22:N22"/>
-    <mergeCell ref="G24:N24"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="O2:Z2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="F3:AC3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="O4:X4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="C2:E3"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="Q37:T37"/>
+    <mergeCell ref="Q38:T38"/>
+    <mergeCell ref="Q39:T39"/>
+    <mergeCell ref="Q41:T41"/>
+    <mergeCell ref="Q40:T40"/>
+    <mergeCell ref="Q42:T42"/>
+    <mergeCell ref="Q44:T44"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="Q45:T45"/>
+    <mergeCell ref="Q46:T46"/>
+    <mergeCell ref="Q47:T47"/>
+    <mergeCell ref="Q48:T48"/>
+    <mergeCell ref="Q49:T49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>